<commit_message>
Added final powerpoint and excel
</commit_message>
<xml_diff>
--- a/Results for Replication of A Large-Scale Car Dataset for Fine-Grained Categorization and Verification.xlsx
+++ b/Results for Replication of A Large-Scale Car Dataset for Fine-Grained Categorization and Verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\car_prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Documents/GitHub/car_prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EDB209-336C-4520-B8BC-7DAC91082D98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CFD49A-9C1D-174A-8C90-1751EEF4A18A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{2AD8FAAC-749C-1443-9559-2BD61E00ABCB}"/>
+    <workbookView xWindow="-120" yWindow="460" windowWidth="38640" windowHeight="16800" activeTab="1" xr2:uid="{2AD8FAAC-749C-1443-9559-2BD61E00ABCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Results" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="34">
   <si>
     <t>Results of Replication of A Large-Scale Car Dataset for Fine-Grained Categorization and Verification</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>Softmax</t>
+  </si>
+  <si>
+    <t>Best SVM</t>
+  </si>
+  <si>
+    <t>Divide learning rate by 5 every 50 epochs</t>
+  </si>
+  <si>
+    <t>~50</t>
+  </si>
+  <si>
+    <t>Best Softmax</t>
   </si>
 </sst>
 </file>
@@ -142,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +164,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -348,6 +372,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,27 +697,27 @@
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="7" max="7" width="20.875" customWidth="1"/>
-    <col min="12" max="12" width="29.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="12" max="12" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" customWidth="1"/>
     <col min="14" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="16" width="16.875" customWidth="1"/>
-    <col min="17" max="17" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="16.83203125" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.625" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -696,7 +725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -718,7 +747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
@@ -744,7 +773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
@@ -770,7 +799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
@@ -799,35 +828,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A26EB79-3F41-7041-863F-F8F5D77CB66D}">
-  <dimension ref="B3:N12"/>
+  <dimension ref="A3:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26:N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -868,232 +897,250 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5">
-        <v>152807</v>
+        <v>3563</v>
       </c>
       <c r="D5">
-        <v>38202</v>
-      </c>
-      <c r="E5">
-        <v>21224</v>
-      </c>
-      <c r="F5">
-        <v>20000</v>
+        <v>891</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
       </c>
       <c r="G5">
+        <v>1E-4</v>
+      </c>
+      <c r="H5">
+        <v>50</v>
+      </c>
+      <c r="I5">
         <v>0.1</v>
-      </c>
-      <c r="H5">
-        <v>200</v>
-      </c>
-      <c r="I5">
-        <v>1E-3</v>
       </c>
       <c r="J5" t="s">
         <v>27</v>
       </c>
       <c r="K5">
-        <v>65.502888999999996</v>
-      </c>
-      <c r="L5">
-        <v>65.658866000000003</v>
-      </c>
-      <c r="M5">
-        <v>65.105541000000002</v>
-      </c>
-      <c r="N5">
-        <v>47.88</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6">
-        <v>152807</v>
+        <v>3563</v>
       </c>
       <c r="D6">
-        <v>38202</v>
-      </c>
-      <c r="E6">
-        <v>21224</v>
-      </c>
-      <c r="F6">
-        <v>20000</v>
+        <v>891</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
       </c>
       <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
         <v>0.1</v>
       </c>
-      <c r="H6">
-        <v>200</v>
-      </c>
-      <c r="I6">
-        <v>0.01</v>
-      </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K6">
-        <v>54.583232000000002</v>
-      </c>
-      <c r="L6">
-        <v>54.324381000000002</v>
-      </c>
-      <c r="M6">
-        <v>54.584432999999997</v>
-      </c>
-      <c r="N6">
-        <v>50.305</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+        <v>79.2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7">
-        <v>152807</v>
+        <v>3563</v>
       </c>
       <c r="D7">
-        <v>38202</v>
-      </c>
-      <c r="E7">
-        <v>21224</v>
-      </c>
-      <c r="F7">
-        <v>20000</v>
+        <v>891</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
       </c>
       <c r="G7">
+        <v>0.01</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="I7">
         <v>0.1</v>
       </c>
-      <c r="H7">
-        <v>200</v>
-      </c>
-      <c r="I7">
-        <v>0.01</v>
-      </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7">
-        <v>59.034599</v>
+        <v>75.28</v>
       </c>
       <c r="L7">
-        <v>59.470708000000002</v>
-      </c>
-      <c r="M7">
-        <v>58.989823000000001</v>
-      </c>
-      <c r="N7">
-        <v>49.51</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+        <v>73.09</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8">
-        <v>152807</v>
+        <v>3563</v>
       </c>
       <c r="D8">
-        <v>38202</v>
-      </c>
-      <c r="E8">
-        <v>21224</v>
-      </c>
-      <c r="F8">
-        <v>20000</v>
+        <v>891</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
       </c>
       <c r="G8">
         <v>0.01</v>
       </c>
       <c r="H8">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="I8">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="J8" t="s">
         <v>27</v>
       </c>
       <c r="K8">
-        <v>51.857571999999998</v>
+        <v>81.8</v>
       </c>
       <c r="L8">
-        <v>51.670070000000003</v>
-      </c>
-      <c r="M8">
-        <v>51.865811999999998</v>
-      </c>
-      <c r="N8">
-        <v>51.435000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+        <v>77.8</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
       <c r="C9">
-        <v>152807</v>
+        <v>3563</v>
       </c>
       <c r="D9">
-        <v>38202</v>
-      </c>
-      <c r="E9">
-        <v>21224</v>
-      </c>
-      <c r="F9">
-        <v>20000</v>
+        <v>891</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
       </c>
       <c r="G9">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="H9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I9">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="J9" t="s">
         <v>27</v>
       </c>
       <c r="K9">
-        <v>55.893382000000003</v>
+        <v>86.29</v>
       </c>
       <c r="L9">
-        <v>56.455159000000002</v>
-      </c>
-      <c r="M9">
-        <v>55.639842000000002</v>
-      </c>
-      <c r="N9">
-        <v>48.89</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+        <v>78.7</v>
+      </c>
+      <c r="M9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>152807</v>
+        <v>3563</v>
       </c>
       <c r="D10">
-        <v>38202</v>
-      </c>
-      <c r="E10">
-        <v>21224</v>
-      </c>
-      <c r="F10">
-        <v>20000</v>
+        <v>891</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
       </c>
       <c r="G10">
         <v>0.1</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I10">
         <v>0.01</v>
@@ -1102,76 +1149,730 @@
         <v>27</v>
       </c>
       <c r="K10">
-        <v>65.131833</v>
+        <v>92.13</v>
       </c>
       <c r="L10">
-        <v>65.517511999999996</v>
-      </c>
-      <c r="M10">
-        <v>64.705050999999997</v>
-      </c>
-      <c r="N10">
-        <v>48.02</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+        <v>84.08</v>
+      </c>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>152807</v>
+        <v>3563</v>
       </c>
       <c r="D11">
-        <v>38202</v>
-      </c>
-      <c r="E11">
-        <v>21224</v>
-      </c>
-      <c r="F11">
-        <v>20000</v>
+        <v>891</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
       </c>
       <c r="G11">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="H11">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I11">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="J11" t="s">
         <v>27</v>
       </c>
       <c r="K11">
+        <v>91.91</v>
+      </c>
+      <c r="L11">
+        <v>83.63</v>
+      </c>
+      <c r="M11" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>3563</v>
+      </c>
+      <c r="D12">
+        <v>891</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>0.1</v>
+      </c>
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <v>1E-4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12">
+        <v>91.63</v>
+      </c>
+      <c r="L12">
+        <v>83.86</v>
+      </c>
+      <c r="M12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="13">
+        <v>3563</v>
+      </c>
+      <c r="D13" s="13">
+        <v>891</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="13">
+        <v>100</v>
+      </c>
+      <c r="I13" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="13">
+        <v>88.54</v>
+      </c>
+      <c r="L13" s="13">
+        <v>86.1</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="13"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>3563</v>
+      </c>
+      <c r="D14">
+        <v>891</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>0.01</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <v>0.1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14">
+        <v>73.39</v>
+      </c>
+      <c r="L14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>3563</v>
+      </c>
+      <c r="D15">
+        <v>891</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>0.01</v>
+      </c>
+      <c r="H15">
+        <v>100</v>
+      </c>
+      <c r="I15">
+        <v>0.1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15">
+        <v>89.94</v>
+      </c>
+      <c r="L15">
+        <v>88.57</v>
+      </c>
+      <c r="M15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>3563</v>
+      </c>
+      <c r="D16">
+        <v>891</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>0.01</v>
+      </c>
+      <c r="H16">
+        <v>100</v>
+      </c>
+      <c r="I16">
+        <v>0.01</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16">
+        <v>89.55</v>
+      </c>
+      <c r="L16">
+        <v>89.46</v>
+      </c>
+      <c r="M16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>3563</v>
+      </c>
+      <c r="D17">
+        <v>891</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>0.1</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
+      <c r="I17">
+        <v>0.01</v>
+      </c>
+      <c r="J17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17">
+        <v>90.45</v>
+      </c>
+      <c r="L17">
+        <v>86.32</v>
+      </c>
+      <c r="M17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>3563</v>
+      </c>
+      <c r="D18">
+        <v>891</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>1E-3</v>
+      </c>
+      <c r="H18">
+        <v>100</v>
+      </c>
+      <c r="I18">
+        <v>0.01</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18">
+        <v>85.28</v>
+      </c>
+      <c r="L18">
+        <v>87.22</v>
+      </c>
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
+        <v>15</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="13">
+        <v>3563</v>
+      </c>
+      <c r="D19" s="13">
+        <v>891</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="13">
+        <v>100</v>
+      </c>
+      <c r="I19" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="13">
+        <v>89.66</v>
+      </c>
+      <c r="L19" s="13">
+        <v>89.24</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
+        <v>16</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="13">
+        <v>152807</v>
+      </c>
+      <c r="D20" s="13">
+        <v>38202</v>
+      </c>
+      <c r="E20" s="13">
+        <v>21224</v>
+      </c>
+      <c r="F20" s="13">
+        <v>20000</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="13">
+        <v>200</v>
+      </c>
+      <c r="I20" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="13">
+        <v>65.502888999999996</v>
+      </c>
+      <c r="L20" s="13">
+        <v>65.658866000000003</v>
+      </c>
+      <c r="M20" s="13">
+        <v>65.105541000000002</v>
+      </c>
+      <c r="N20" s="13">
+        <v>47.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>152807</v>
+      </c>
+      <c r="D21">
+        <v>38202</v>
+      </c>
+      <c r="E21">
+        <v>21224</v>
+      </c>
+      <c r="F21">
+        <v>20000</v>
+      </c>
+      <c r="G21">
+        <v>0.1</v>
+      </c>
+      <c r="H21">
+        <v>200</v>
+      </c>
+      <c r="I21">
+        <v>0.01</v>
+      </c>
+      <c r="J21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21">
+        <v>54.583232000000002</v>
+      </c>
+      <c r="L21">
+        <v>54.324381000000002</v>
+      </c>
+      <c r="M21">
+        <v>54.584432999999997</v>
+      </c>
+      <c r="N21">
+        <v>50.305</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>152807</v>
+      </c>
+      <c r="D22">
+        <v>38202</v>
+      </c>
+      <c r="E22">
+        <v>21224</v>
+      </c>
+      <c r="F22">
+        <v>20000</v>
+      </c>
+      <c r="G22">
+        <v>0.1</v>
+      </c>
+      <c r="H22">
+        <v>200</v>
+      </c>
+      <c r="I22">
+        <v>0.01</v>
+      </c>
+      <c r="J22" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22">
+        <v>59.034599</v>
+      </c>
+      <c r="L22">
+        <v>59.470708000000002</v>
+      </c>
+      <c r="M22">
+        <v>58.989823000000001</v>
+      </c>
+      <c r="N22">
+        <v>49.51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>152807</v>
+      </c>
+      <c r="D23">
+        <v>38202</v>
+      </c>
+      <c r="E23">
+        <v>21224</v>
+      </c>
+      <c r="F23">
+        <v>20000</v>
+      </c>
+      <c r="G23">
+        <v>0.01</v>
+      </c>
+      <c r="H23">
+        <v>200</v>
+      </c>
+      <c r="I23">
+        <v>0.01</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23">
+        <v>51.857571999999998</v>
+      </c>
+      <c r="L23">
+        <v>51.670070000000003</v>
+      </c>
+      <c r="M23">
+        <v>51.865811999999998</v>
+      </c>
+      <c r="N23">
+        <v>51.435000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>152807</v>
+      </c>
+      <c r="D24">
+        <v>38202</v>
+      </c>
+      <c r="E24">
+        <v>21224</v>
+      </c>
+      <c r="F24">
+        <v>20000</v>
+      </c>
+      <c r="G24">
+        <v>0.01</v>
+      </c>
+      <c r="H24">
+        <v>50</v>
+      </c>
+      <c r="I24">
+        <v>0.01</v>
+      </c>
+      <c r="J24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24">
+        <v>55.893382000000003</v>
+      </c>
+      <c r="L24">
+        <v>56.455159000000002</v>
+      </c>
+      <c r="M24">
+        <v>55.639842000000002</v>
+      </c>
+      <c r="N24">
+        <v>48.89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>152807</v>
+      </c>
+      <c r="D25">
+        <v>38202</v>
+      </c>
+      <c r="E25">
+        <v>21224</v>
+      </c>
+      <c r="F25">
+        <v>20000</v>
+      </c>
+      <c r="G25">
+        <v>0.1</v>
+      </c>
+      <c r="H25">
+        <v>50</v>
+      </c>
+      <c r="I25">
+        <v>0.01</v>
+      </c>
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25">
+        <v>65.131833</v>
+      </c>
+      <c r="L25">
+        <v>65.517511999999996</v>
+      </c>
+      <c r="M25">
+        <v>64.705050999999997</v>
+      </c>
+      <c r="N25">
+        <v>48.02</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13">
+        <v>22</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="13">
+        <v>152807</v>
+      </c>
+      <c r="D26" s="13">
+        <v>38202</v>
+      </c>
+      <c r="E26" s="13">
+        <v>21224</v>
+      </c>
+      <c r="F26" s="13">
+        <v>20000</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="H26" s="13">
+        <v>50</v>
+      </c>
+      <c r="I26" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="13">
         <v>65.111546000000004</v>
       </c>
-      <c r="L11">
+      <c r="L26" s="13">
         <v>65.452071000000004</v>
       </c>
-      <c r="M11">
+      <c r="M26" s="13">
         <v>64.780437000000006</v>
       </c>
-      <c r="N11">
+      <c r="N26" s="13">
         <v>47.66</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12">
-        <v>152807</v>
-      </c>
-      <c r="D12">
-        <v>38202</v>
-      </c>
-      <c r="E12">
-        <v>21224</v>
-      </c>
-      <c r="F12">
-        <v>20000</v>
-      </c>
-    </row>
+    <row r="27" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>